<commit_message>
Commit :2. This is Hybrid framework With Implementation
</commit_message>
<xml_diff>
--- a/HybridFramework_LP/TestInPut/HybridTest.xlsx
+++ b/HybridFramework_LP/TestInPut/HybridTest.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srikanth\eclipse-workspace\HybridFramework_LP\TestInPut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srikanth\git\Hybridframework_LP\HybridFramework_LP\TestInPut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1A72B40-7D33-44AB-B7CD-39B55D076E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43DC700-4234-476A-8C75-40548DB6C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A7A9517F-180B-4E87-960F-9A7A391D0B46}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{74F885E5-03D2-4CFA-8AF0-85D38F688125}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="ApplicationLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,22 +34,169 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Result</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>ModuleName</t>
+  </si>
+  <si>
+    <t>ExecutionMode</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>ApplicationLogin</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>StockCategories</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ObjectiveType</t>
+  </si>
+  <si>
+    <t>LocatorType</t>
+  </si>
+  <si>
+    <t>LocatorValue</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Launch Browser</t>
+  </si>
+  <si>
+    <t>startBrowser</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Launch application url</t>
+  </si>
+  <si>
+    <t>openApplication</t>
+  </si>
+  <si>
+    <t>wait for username</t>
+  </si>
+  <si>
+    <t>waitForElement</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Enter username</t>
+  </si>
+  <si>
+    <t>typeAction</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>wait for password</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>wait for login button</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//button[@id='btnsubmit']</t>
+  </si>
+  <si>
+    <t>Click on login button</t>
+  </si>
+  <si>
+    <t>clickAction</t>
+  </si>
+  <si>
+    <t>wait for logout link</t>
+  </si>
+  <si>
+    <t>//a[@id='logout']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify title </t>
+  </si>
+  <si>
+    <t>validateTitle</t>
+  </si>
+  <si>
+    <t>Dashboard « Stock Accounting</t>
+  </si>
+  <si>
+    <t>click logout link</t>
+  </si>
+  <si>
+    <t>wait for alert ok button</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'OK!')]</t>
+  </si>
+  <si>
+    <t>click alert ok button</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,13 +204,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -83,9 +252,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,20 +570,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B150689-FD35-448C-8FB2-380E02164DB8}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837061DC-0A32-4239-82FA-BF2D1B846A6A}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,6 +593,348 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E6A687-F574-4DB9-8D33-9584C1A99DA4}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>